<commit_message>
get an update in ya
</commit_message>
<xml_diff>
--- a/dataformat.xlsx
+++ b/dataformat.xlsx
@@ -155,13 +155,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,7 +467,7 @@
   <dimension ref="B2:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,11 +483,11 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
@@ -760,7 +761,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>